<commit_message>
mortalidad y produccion de leche
</commit_message>
<xml_diff>
--- a/data/transmision verticas.xlsx
+++ b/data/transmision verticas.xlsx
@@ -36,6 +36,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,7 +90,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -103,22 +106,15 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -548,7 +544,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +657,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="6"/>
+      <c r="B17" s="8"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18"/>
@@ -702,52 +698,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="cellIs" dxfId="15" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="59" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="14" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="58" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="13" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="53" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="12" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="48" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="11" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="41" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="10" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="37" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="cellIs" dxfId="9" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="31" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="cellIs" dxfId="8" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="30" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="cellIs" dxfId="7" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="27" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="cellIs" dxfId="6" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="24" operator="greaterThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>